<commit_message>
make the buttons for feedback and github similar to rainfall calculator
</commit_message>
<xml_diff>
--- a/QA_Documents/QA Data - Auckland Wetland Outlet.xlsx
+++ b/QA_Documents/QA Data - Auckland Wetland Outlet.xlsx
@@ -6400,19 +6400,22 @@
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="15351079-27be-49c5-816a-0df13826569b">
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2">
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="dcf826ae-ce52-4e0f-987a-3ae5dcf3d3c6" xsi:nil="true"/>
+    <TaxCatchAll xmlns="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D5C38F6E58E8684A98E5CD6941DDF6E1" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="46840d43744c05d609145cc701914843">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="15351079-27be-49c5-816a-0df13826569b" xmlns:ns3="dcf826ae-ce52-4e0f-987a-3ae5dcf3d3c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64562b4ca29f62cf0c8cc67afffe8ca1" ns2:_="" ns3:_="">
-    <xsd:import namespace="15351079-27be-49c5-816a-0df13826569b"/>
-    <xsd:import namespace="dcf826ae-ce52-4e0f-987a-3ae5dcf3d3c6"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21cacd0d90dbd8beb6fc12ad84d4cd0e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b418c8325abc32123734ac979891270" ns1:_="" ns2:_="" ns3:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
+    <xsd:import namespace="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
+    <xsd:import namespace="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -6423,16 +6426,19 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -6440,7 +6446,21 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="15351079-27be-49c5-816a-0df13826569b" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="23" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="24" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="02ea596c-bf3f-4512-ad68-024a720c79b2" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -6465,61 +6485,55 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="12" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="17" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="307c9898-a061-40be-acbc-74b50301d7f8" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="21" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceLocation" ma:index="22" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="307c9898-a061-40be-acbc-74b50301d7f8" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="20" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+    <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="21" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="22" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="dcf826ae-ce52-4e0f-987a-3ae5dcf3d3c6" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="17" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c9cc38aa-dbcb-49e2-baa8-e62ab474f760}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="dcf826ae-ce52-4e0f-987a-3ae5dcf3d3c6">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -6538,12 +6552,23 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="20" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{ff3aeec9-456a-4e5c-84fd-d1a0d9fd1185}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="959569b2-1f16-4dd0-b5ed-bb064e5cd07e">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -6668,20 +6693,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FA808F4-436E-47CD-A87A-5A3F09116C33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="15351079-27be-49c5-816a-0df13826569b"/>
-    <ds:schemaRef ds:uri="dcf826ae-ce52-4e0f-987a-3ae5dcf3d3c6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{449E513D-32EF-48B7-8420-ED792615F9F6}"/>
 </file>
</xml_diff>

<commit_message>
Added a button under feedbackform to link the article as requested
</commit_message>
<xml_diff>
--- a/QA_Documents/QA Data - Auckland Wetland Outlet.xlsx
+++ b/QA_Documents/QA Data - Auckland Wetland Outlet.xlsx
@@ -6406,13 +6406,14 @@
     <TaxCatchAll xmlns="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <OldForms xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21cacd0d90dbd8beb6fc12ad84d4cd0e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b418c8325abc32123734ac979891270" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="75e20f4bf570a29fdd68b6ac0ce9f23e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d8333fcdd8157586878df4d15f204f2" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
     <xsd:import namespace="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
@@ -6439,6 +6440,8 @@
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:OldForms" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -6527,6 +6530,18 @@
     <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="26" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OldForms" ma:index="27" nillable="true" ma:displayName="Old Forms " ma:format="Dropdown" ma:internalName="OldForms">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -6693,5 +6708,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{449E513D-32EF-48B7-8420-ED792615F9F6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF466521-89FC-4592-9A98-E41046DEDCCD}"/>
 </file>
</xml_diff>